<commit_message>
use norwegian title if no english jobtitle
</commit_message>
<xml_diff>
--- a/assets/stillingskoder.xlsx
+++ b/assets/stillingskoder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vew002\Workspace\Add-ins\word-add-in\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14892C30-8917-433A-81B4-04F43F5DFA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B20AE2-4B75-4EF6-989A-B1EB41F3D2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EC1E2602-5B5B-4442-905A-93337ED73C01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EC1E2602-5B5B-4442-905A-93337ED73C01}"/>
   </bookViews>
   <sheets>
     <sheet name="stillingskoder" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="289">
   <si>
     <t>SKO</t>
   </si>
@@ -981,8 +981,7 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1003,7 +1002,8 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="right" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1025,18 +1025,18 @@
     <sortCondition ref="D1:D188"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{CAFAD6C6-5701-4FCB-AD81-02ABFCD58898}" name="SKO" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{EE66EF86-D294-4982-BE2C-3DAF163438BA}" name="Norsk" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{CAFAD6C6-5701-4FCB-AD81-02ABFCD58898}" name="SKO" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{EE66EF86-D294-4982-BE2C-3DAF163438BA}" name="Norsk" dataDxfId="6">
       <calculatedColumnFormula>CONCATENATE(stillingskoder[[#This Row],[SKO]]," - ",stillingskoder[[#This Row],[Norsk stillingsbetegnelse]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{20574F42-795B-407A-A3CA-455B2D5855D7}" name="Engelsk" dataDxfId="7">
+    <tableColumn id="6" xr3:uid="{20574F42-795B-407A-A3CA-455B2D5855D7}" name="Engelsk" dataDxfId="5">
       <calculatedColumnFormula>CONCATENATE(stillingskoder[[#This Row],[SKO]]," - ",stillingskoder[[#This Row],[Engelsk stillingsbetegnelse]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E1A0ADBD-C23F-4945-862B-06B735E57D0E}" name="Norsk stillingsbetegnelse" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{398ACFCF-4964-4BE3-9BB8-6EFE9B7A2758}" name="Engelsk stillingsbetegnelse" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{87506794-DC18-4103-BEEA-60916B7A7256}" name="Kategori" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{FBE9E420-6E6D-4A21-BED4-FAB3F256B137}" name="Undervisning" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{802CE78E-6223-4B5D-996F-1678DC3444E3}" name="InUse" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E1A0ADBD-C23F-4945-862B-06B735E57D0E}" name="Norsk stillingsbetegnelse" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{398ACFCF-4964-4BE3-9BB8-6EFE9B7A2758}" name="Engelsk stillingsbetegnelse" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{87506794-DC18-4103-BEEA-60916B7A7256}" name="Kategori" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{FBE9E420-6E6D-4A21-BED4-FAB3F256B137}" name="Undervisning" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{802CE78E-6223-4B5D-996F-1678DC3444E3}" name="InUse" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1362,7 +1362,7 @@
   <dimension ref="A1:H188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1754,10 +1754,13 @@
       </c>
       <c r="C15" t="str">
         <f>CONCATENATE(stillingskoder[[#This Row],[SKO]]," - ",stillingskoder[[#This Row],[Engelsk stillingsbetegnelse]])</f>
-        <v xml:space="preserve">1084 - </v>
+        <v>1084 - Principal Engineer</v>
       </c>
       <c r="D15" t="s">
         <v>69</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
       </c>
       <c r="F15" t="s">
         <v>6</v>

</xml_diff>